<commit_message>
Update to add more database schema with endpoints
</commit_message>
<xml_diff>
--- a/src/main/resources/template.xlsx
+++ b/src/main/resources/template.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/grantyang/IdeaProjects/StoneTicket/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A410CA-0AC1-9B40-8EA5-FE4AB4F63233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BADEB37-72E1-3F48-97DA-06D821FB67EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="12420" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="12420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="welcome" sheetId="1" r:id="rId1"/>
     <sheet name="venue" sheetId="2" r:id="rId2"/>
     <sheet name="venue-layout" sheetId="5" r:id="rId3"/>
     <sheet name="area1 " sheetId="3" r:id="rId4"/>
-    <sheet name="area1-layout" sheetId="6" r:id="rId5"/>
+    <sheet name="area1-seats" sheetId="6" r:id="rId5"/>
     <sheet name="area2" sheetId="4" r:id="rId6"/>
-    <sheet name="area2-layout" sheetId="7" r:id="rId7"/>
+    <sheet name="area2-seats" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="33">
   <si>
     <t xml:space="preserve">Welcome to StoneTicket! </t>
   </si>
@@ -120,6 +120,24 @@
   </si>
   <si>
     <t xml:space="preserve">        var metadata = event.target.getAttribute('metadata');</t>
+  </si>
+  <si>
+    <t>The tab "welcome": no need to parse it for now</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The tab "venue": it is used to record some key value based attribute as name and metadata. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The tab "venue-layout" it is used to draw the graphic layout of different areas in venue. The color of each filled cell will be used to generate a svg image. The content (data) of each cell as index, will be used to refer to to its corresponding area. For example, if the cell content is "2", then this cell belongs to the area in tab names "area-2". </t>
+  </si>
+  <si>
+    <t xml:space="preserve">We can have multiple areas in one venue, so the cell data in tab "venue-layout" will also have multiple corresponding choices. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The tabs "area-{areaId}": are used to save name and metadata of a given area. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The tabs "area-{areaId}-seats": are used to represent seats in this area. Each seat will have its x-axis and y-axix index according its location in the cell of the tab. All seats will have data either "Y" represent there is available seat, or "N" represent there is unavailable seat, empty cell means there is no seat and system don't have to save and deal with these cell. </t>
   </si>
 </sst>
 </file>
@@ -507,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A18"/>
+  <dimension ref="A1:A30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -583,6 +601,36 @@
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -594,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -640,7 +688,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -852,7 +900,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -975,8 +1023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Completed data initialization and basic REST API. Next step: Pricing and Ordering
</commit_message>
<xml_diff>
--- a/src/main/resources/template.xlsx
+++ b/src/main/resources/template.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/grantyang/IdeaProjects/StoneTicket/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BADEB37-72E1-3F48-97DA-06D821FB67EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6778F757-12BA-504B-85FB-1EAAE58BCE6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="12420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="12420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="welcome" sheetId="1" r:id="rId1"/>
     <sheet name="venue" sheetId="2" r:id="rId2"/>
     <sheet name="venue-layout" sheetId="5" r:id="rId3"/>
-    <sheet name="area1 " sheetId="3" r:id="rId4"/>
+    <sheet name="area1" sheetId="3" r:id="rId4"/>
     <sheet name="area1-seats" sheetId="6" r:id="rId5"/>
     <sheet name="area2" sheetId="4" r:id="rId6"/>
     <sheet name="area2-seats" sheetId="7" r:id="rId7"/>
@@ -527,7 +527,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A30"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
@@ -642,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -688,7 +688,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -990,7 +990,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>